<commit_message>
Import excel- WO data
</commit_message>
<xml_diff>
--- a/DOC/LKU_MHE_Master.xlsx
+++ b/DOC/LKU_MHE_Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Master\MMLogistic\MHE_NAV\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B973AF8-F5E2-4116-A3C5-3A162DE50970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353EB6B-D98E-473A-B575-53E02347F418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,6 +519,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="187" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -558,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,6 +593,7 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,7 +930,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -939,11 +943,11 @@
     <col min="6" max="6" width="11.54296875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="9" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.453125" customWidth="1"/>
     <col min="13" max="13" width="18.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="18.81640625" customWidth="1"/>
     <col min="18" max="18" width="9.08984375" customWidth="1"/>
@@ -1613,7 +1617,7 @@
       </c>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>9334</v>
       </c>
@@ -1672,7 +1676,7 @@
       </c>
       <c r="U12" s="8"/>
     </row>
-    <row r="13" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>9335</v>
       </c>
@@ -1731,7 +1735,7 @@
       </c>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>9336</v>
       </c>
@@ -1790,7 +1794,7 @@
       </c>
       <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>9337</v>
       </c>
@@ -1847,7 +1851,7 @@
       <c r="T15" s="5"/>
       <c r="U15" s="8"/>
     </row>
-    <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>9338</v>
       </c>
@@ -1906,7 +1910,7 @@
       </c>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>9339</v>
       </c>
@@ -1963,7 +1967,7 @@
       <c r="T17" s="5"/>
       <c r="U17" s="8"/>
     </row>
-    <row r="18" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>9340</v>
       </c>
@@ -2022,7 +2026,7 @@
       </c>
       <c r="U18" s="8"/>
     </row>
-    <row r="19" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>9341</v>
       </c>
@@ -2079,7 +2083,7 @@
       <c r="T19" s="5"/>
       <c r="U19" s="8"/>
     </row>
-    <row r="20" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>9342</v>
       </c>
@@ -7369,48 +7373,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735E1BE8-12B0-4379-AB73-7AC2C6995656}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I3" sqref="I3:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>155</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I1" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J1" s="13">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I2" s="11">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I3" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>162</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.64583333333333304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="11">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I6" s="11">
+        <v>0.687499999999999</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0.687499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I7" s="11">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.70833333333333304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I8" s="11">
+        <v>0.72916666666666596</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.72916666666666596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I9" s="11">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0.749999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I10" s="11">
+        <v>0.77083333333333204</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0.77083333333333204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I11" s="11">
+        <v>0.79166666666666596</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.79166666666666596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I12" s="11">
+        <v>0.812499999999999</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0.812499999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I13" s="11">
+        <v>0.83333333333333204</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.83333333333333204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I14" s="11">
+        <v>0.85416666666666496</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.85416666666666496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I15" s="11">
+        <v>0.874999999999999</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.874999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I16" s="11">
+        <v>0.89583333333333204</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0.89583333333333204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create WO from List
</commit_message>
<xml_diff>
--- a/DOC/LKU_MHE_Master.xlsx
+++ b/DOC/LKU_MHE_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Master\MMLogistic\MHE_NAV\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353EB6B-D98E-473A-B575-53E02347F418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC8204B-015D-4DE1-9DFC-EDED2FA3EFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,7 +930,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Driver Sub -Job task
</commit_message>
<xml_diff>
--- a/DOC/LKU_MHE_Master.xlsx
+++ b/DOC/LKU_MHE_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Master\MMLogistic\MHE_NAV\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC8204B-015D-4DE1-9DFC-EDED2FA3EFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9556D497-96B4-4242-818D-3380DBB3F07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FleetMe_Task" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,6 +594,25 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2256,64 +2275,64 @@
       </c>
       <c r="U22" s="8"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+    <row r="23" spans="1:21" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14">
         <v>9345</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="15">
         <v>44971</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="17">
         <v>0.3125</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="17">
         <v>0.6875</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="N23" s="7" t="s">
+      <c r="N23" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="P23" s="5" t="s">
+      <c r="P23" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5" t="s">
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="T23" s="5" t="s">
+      <c r="T23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="U23" s="8"/>
+      <c r="U23" s="19"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
@@ -7364,9 +7383,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>